<commit_message>
Mental health headings ECENQS notes/sources fix.
</commit_message>
<xml_diff>
--- a/dashboard_loader/education_ecenqs_uploader/education_ecenqs.xlsx
+++ b/dashboard_loader/education_ecenqs_uploader/education_ecenqs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -102,13 +102,13 @@
     <t xml:space="preserve">Performance against benchmarks are expressed as a percentage of the number of services as at 30 June 2015.</t>
   </si>
   <si>
+    <t xml:space="preserve">This figure does not include services that received a rating of ‘significant improvement required’. At the end of September 2013 there were nine services that received the rating ‘significant improvement required’ and at the end of September 2016 there were 21 services that had this rating.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Source</t>
   </si>
   <si>
     <t xml:space="preserve">Australian Children’s Education and Care Quality Authority NQF Snapshot Q1-2013, Q3-2015, Q3-2016, Q4-2017.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This figure does not include services that received a rating of ‘significant improvement required’. At the end of September 2013 there were nine services that received the rating ‘significant improvement required’ and at the end of September 2016 there were 21 services that had this rating.</t>
   </si>
 </sst>
 </file>
@@ -280,7 +280,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -325,10 +325,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -337,10 +333,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -358,10 +350,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -476,7 +464,7 @@
   </sheetPr>
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="M25" activeCellId="0" sqref="M25"/>
     </sheetView>
   </sheetViews>
@@ -591,19 +579,19 @@
       <c r="H5" s="10" t="n">
         <v>928</v>
       </c>
-      <c r="I5" s="11" t="n">
+      <c r="I5" s="10" t="n">
         <v>1029</v>
       </c>
-      <c r="J5" s="11" t="n">
+      <c r="J5" s="10" t="n">
         <v>197</v>
       </c>
-      <c r="K5" s="11" t="n">
+      <c r="K5" s="10" t="n">
         <v>261</v>
       </c>
-      <c r="L5" s="11" t="n">
+      <c r="L5" s="10" t="n">
         <v>149</v>
       </c>
-      <c r="M5" s="11" t="n">
+      <c r="M5" s="10" t="n">
         <v>11266</v>
       </c>
       <c r="N5" s="3"/>
@@ -611,35 +599,35 @@
     <row r="6" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7"/>
       <c r="B6" s="5"/>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="5"/>
-      <c r="E6" s="13" t="n">
+      <c r="E6" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="F6" s="13" t="n">
+      <c r="F6" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="G6" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="14" t="n">
+      <c r="G6" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="J6" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="L6" s="14" t="n">
+      <c r="J6" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="M6" s="14" t="n">
+      <c r="M6" s="12" t="n">
         <v>9</v>
       </c>
       <c r="N6" s="3"/>
@@ -662,19 +650,19 @@
       <c r="H7" s="10" t="n">
         <v>28</v>
       </c>
-      <c r="I7" s="11" t="n">
+      <c r="I7" s="10" t="n">
         <v>27</v>
       </c>
-      <c r="J7" s="11" t="n">
+      <c r="J7" s="10" t="n">
         <v>17</v>
       </c>
-      <c r="K7" s="11" t="n">
+      <c r="K7" s="10" t="n">
         <v>33</v>
       </c>
-      <c r="L7" s="11" t="n">
+      <c r="L7" s="10" t="n">
         <v>37</v>
       </c>
-      <c r="M7" s="11" t="n">
+      <c r="M7" s="10" t="n">
         <v>710</v>
       </c>
       <c r="N7" s="3"/>
@@ -697,19 +685,19 @@
       <c r="H8" s="10" t="n">
         <v>9</v>
       </c>
-      <c r="I8" s="11" t="n">
+      <c r="I8" s="10" t="n">
         <v>60</v>
       </c>
-      <c r="J8" s="11" t="n">
+      <c r="J8" s="10" t="n">
         <v>9</v>
       </c>
-      <c r="K8" s="11" t="n">
+      <c r="K8" s="10" t="n">
         <v>13</v>
       </c>
-      <c r="L8" s="11" t="n">
+      <c r="L8" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="M8" s="15" t="n">
+      <c r="M8" s="13" t="n">
         <v>901</v>
       </c>
       <c r="N8" s="3"/>
@@ -718,19 +706,19 @@
       <c r="B9" s="3"/>
       <c r="C9" s="8"/>
       <c r="D9" s="9"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
       <c r="N9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="17"/>
+      <c r="B10" s="15"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
@@ -782,10 +770,10 @@
     </row>
     <row r="12" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="5"/>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="18"/>
+      <c r="D12" s="16"/>
       <c r="E12" s="10" t="n">
         <v>8</v>
       </c>
@@ -810,7 +798,7 @@
       <c r="L12" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="M12" s="11" t="n">
+      <c r="M12" s="10" t="n">
         <v>9</v>
       </c>
     </row>
@@ -883,16 +871,16 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="17"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="16"/>
+      <c r="B15" s="15"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="n">
@@ -903,40 +891,40 @@
         <v>10</v>
       </c>
       <c r="D16" s="9"/>
-      <c r="E16" s="11" t="n">
+      <c r="E16" s="10" t="n">
         <v>1075</v>
       </c>
-      <c r="F16" s="11" t="n">
+      <c r="F16" s="10" t="n">
         <v>360</v>
       </c>
-      <c r="G16" s="11" t="n">
+      <c r="G16" s="10" t="n">
         <v>350</v>
       </c>
-      <c r="H16" s="11" t="n">
+      <c r="H16" s="10" t="n">
         <v>330</v>
       </c>
-      <c r="I16" s="11" t="n">
+      <c r="I16" s="10" t="n">
         <v>450</v>
       </c>
-      <c r="J16" s="11" t="n">
+      <c r="J16" s="10" t="n">
         <v>11</v>
       </c>
-      <c r="K16" s="11" t="n">
+      <c r="K16" s="10" t="n">
         <v>49</v>
       </c>
-      <c r="L16" s="11" t="n">
+      <c r="L16" s="10" t="n">
         <v>17</v>
       </c>
-      <c r="M16" s="11" t="n">
+      <c r="M16" s="10" t="n">
         <v>2642</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="5"/>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="18"/>
+      <c r="D17" s="16"/>
       <c r="E17" s="10" t="n">
         <v>9</v>
       </c>
@@ -961,7 +949,7 @@
       <c r="L17" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="M17" s="19" t="n">
+      <c r="M17" s="17" t="n">
         <v>21</v>
       </c>
     </row>
@@ -971,31 +959,31 @@
         <v>12</v>
       </c>
       <c r="D18" s="9"/>
-      <c r="E18" s="11" t="n">
+      <c r="E18" s="10" t="n">
         <v>1460</v>
       </c>
-      <c r="F18" s="11" t="n">
+      <c r="F18" s="10" t="n">
         <v>723</v>
       </c>
-      <c r="G18" s="11" t="n">
+      <c r="G18" s="10" t="n">
         <v>605</v>
       </c>
-      <c r="H18" s="11" t="n">
+      <c r="H18" s="10" t="n">
         <v>316</v>
       </c>
-      <c r="I18" s="11" t="n">
+      <c r="I18" s="10" t="n">
         <v>235</v>
       </c>
-      <c r="J18" s="11" t="n">
+      <c r="J18" s="10" t="n">
         <v>57</v>
       </c>
-      <c r="K18" s="11" t="n">
+      <c r="K18" s="10" t="n">
         <v>124</v>
       </c>
-      <c r="L18" s="11" t="n">
+      <c r="L18" s="10" t="n">
         <v>111</v>
       </c>
-      <c r="M18" s="11" t="n">
+      <c r="M18" s="10" t="n">
         <v>3631</v>
       </c>
     </row>
@@ -1005,58 +993,49 @@
         <v>13</v>
       </c>
       <c r="D19" s="9"/>
-      <c r="E19" s="11" t="n">
+      <c r="E19" s="10" t="n">
         <v>2817</v>
       </c>
-      <c r="F19" s="11" t="n">
+      <c r="F19" s="10" t="n">
         <v>3003</v>
       </c>
-      <c r="G19" s="11" t="n">
+      <c r="G19" s="10" t="n">
         <v>1906</v>
       </c>
-      <c r="H19" s="11" t="n">
+      <c r="H19" s="10" t="n">
         <v>496</v>
       </c>
-      <c r="I19" s="11" t="n">
+      <c r="I19" s="10" t="n">
         <v>478</v>
       </c>
-      <c r="J19" s="11" t="n">
+      <c r="J19" s="10" t="n">
         <v>163</v>
       </c>
-      <c r="K19" s="11" t="n">
+      <c r="K19" s="10" t="n">
         <v>181</v>
       </c>
-      <c r="L19" s="11" t="n">
+      <c r="L19" s="10" t="n">
         <v>91</v>
       </c>
-      <c r="M19" s="11" t="n">
+      <c r="M19" s="10" t="n">
         <v>9135</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="3"/>
       <c r="C20" s="8"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="20"/>
-      <c r="M20" s="20"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="17"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="21"/>
-      <c r="L21" s="21"/>
-      <c r="M21" s="21"/>
+      <c r="B21" s="15"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="n">
@@ -1066,64 +1045,64 @@
       <c r="C22" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="22" t="n">
+      <c r="E22" s="19" t="n">
         <v>207</v>
       </c>
-      <c r="F22" s="22" t="n">
+      <c r="F22" s="19" t="n">
         <v>325</v>
       </c>
-      <c r="G22" s="22" t="n">
+      <c r="G22" s="19" t="n">
         <v>141</v>
       </c>
-      <c r="H22" s="22" t="n">
+      <c r="H22" s="19" t="n">
         <v>85</v>
       </c>
-      <c r="I22" s="22" t="n">
+      <c r="I22" s="19" t="n">
         <v>124</v>
       </c>
-      <c r="J22" s="22" t="n">
+      <c r="J22" s="19" t="n">
         <v>11</v>
       </c>
-      <c r="K22" s="22" t="n">
+      <c r="K22" s="19" t="n">
         <v>35</v>
       </c>
-      <c r="L22" s="22" t="n">
+      <c r="L22" s="19" t="n">
         <v>13</v>
       </c>
-      <c r="M22" s="22" t="n">
+      <c r="M22" s="19" t="n">
         <v>941</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="5"/>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E23" s="22" t="n">
+      <c r="E23" s="19" t="n">
         <v>27</v>
       </c>
-      <c r="F23" s="22" t="n">
+      <c r="F23" s="19" t="n">
         <v>9</v>
       </c>
-      <c r="G23" s="22" t="n">
+      <c r="G23" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="H23" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="I23" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="J23" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="K23" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="L23" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="M23" s="22" t="n">
+      <c r="H23" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" s="19" t="n">
         <v>38</v>
       </c>
     </row>
@@ -1132,31 +1111,31 @@
       <c r="C24" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E24" s="22" t="n">
+      <c r="E24" s="19" t="n">
         <v>1357</v>
       </c>
-      <c r="F24" s="22" t="n">
+      <c r="F24" s="19" t="n">
         <v>635</v>
       </c>
-      <c r="G24" s="22" t="n">
+      <c r="G24" s="19" t="n">
         <v>524</v>
       </c>
-      <c r="H24" s="22" t="n">
+      <c r="H24" s="19" t="n">
         <v>369</v>
       </c>
-      <c r="I24" s="22" t="n">
+      <c r="I24" s="19" t="n">
         <v>286</v>
       </c>
-      <c r="J24" s="22" t="n">
+      <c r="J24" s="19" t="n">
         <v>47</v>
       </c>
-      <c r="K24" s="22" t="n">
+      <c r="K24" s="19" t="n">
         <v>97</v>
       </c>
-      <c r="L24" s="22" t="n">
+      <c r="L24" s="19" t="n">
         <v>81</v>
       </c>
-      <c r="M24" s="22" t="n">
+      <c r="M24" s="19" t="n">
         <v>3396</v>
       </c>
     </row>
@@ -1165,31 +1144,31 @@
       <c r="C25" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E25" s="22" t="n">
+      <c r="E25" s="19" t="n">
         <v>3775</v>
       </c>
-      <c r="F25" s="22" t="n">
+      <c r="F25" s="19" t="n">
         <v>3264</v>
       </c>
-      <c r="G25" s="22" t="n">
+      <c r="G25" s="19" t="n">
         <v>2233</v>
       </c>
-      <c r="H25" s="22" t="n">
+      <c r="H25" s="19" t="n">
         <v>703</v>
       </c>
-      <c r="I25" s="22" t="n">
+      <c r="I25" s="19" t="n">
         <v>752</v>
       </c>
-      <c r="J25" s="22" t="n">
+      <c r="J25" s="19" t="n">
         <v>175</v>
       </c>
-      <c r="K25" s="22" t="n">
+      <c r="K25" s="19" t="n">
         <v>222</v>
       </c>
-      <c r="L25" s="22" t="n">
+      <c r="L25" s="19" t="n">
         <v>129</v>
       </c>
-      <c r="M25" s="22" t="n">
+      <c r="M25" s="19" t="n">
         <v>11253</v>
       </c>
     </row>
@@ -1226,10 +1205,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1240,74 +1219,74 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="21" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="22" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="23" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="27" t="n">
+      <c r="B4" s="24" t="n">
         <v>2017</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="24" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="23"/>
-      <c r="B6" s="26" t="s">
+      <c r="A6" s="20"/>
+      <c r="B6" s="23" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="23" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" customFormat="false" ht="39.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="20"/>
+      <c r="B8" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="26" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="23"/>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="23" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Education NQS text update.
</commit_message>
<xml_diff>
--- a/dashboard_loader/education_ecenqs_uploader/education_ecenqs.xlsx
+++ b/dashboard_loader/education_ecenqs_uploader/education_ecenqs.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t xml:space="preserve">The number of early childhood education and care services in Australia with a quality rating, by quality rating level and jurisdiction, March 2013, September 2015, September 2016, December 2017.</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t xml:space="preserve">This figure does not include services that received a rating of ‘significant improvement required’. At the end of September 2013 there were nine services that received the rating ‘significant improvement required’ and at the end of September 2016 there were 21 services that had this rating.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The NQS commenced implementation in 2013, reflecting low proportions of services assessed for that year.</t>
   </si>
   <si>
     <t xml:space="preserve">Source</t>
@@ -123,7 +126,7 @@
     <numFmt numFmtId="168" formatCode="0.0"/>
     <numFmt numFmtId="169" formatCode="@"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -233,6 +236,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -280,7 +289,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -383,6 +392,10 @@
     </xf>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1205,10 +1218,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1278,15 +1291,21 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="20"/>
+      <c r="B9" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="23" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="B10" s="23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
ECE NQS text change.
</commit_message>
<xml_diff>
--- a/dashboard_loader/education_ecenqs_uploader/education_ecenqs.xlsx
+++ b/dashboard_loader/education_ecenqs_uploader/education_ecenqs.xlsx
@@ -105,7 +105,7 @@
     <t xml:space="preserve">This figure does not include services that received a rating of ‘significant improvement required’. At the end of September 2013 there were nine services that received the rating ‘significant improvement required’ and at the end of September 2016 there were 21 services that had this rating.</t>
   </si>
   <si>
-    <t xml:space="preserve">The NQS commenced implementation in 2013, reflecting low proportions of services assessed for that year.</t>
+    <t xml:space="preserve">The NQS commenced implementation in 2013, which is reflected in low proportions of services assessed for that year.</t>
   </si>
   <si>
     <t xml:space="preserve">Source</t>
@@ -1221,7 +1221,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>